<commit_message>
Built: write commands of import/export user table
</commit_message>
<xml_diff>
--- a/public/csv/exportUsers.xlsx
+++ b/public/csv/exportUsers.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="137">
   <si>
     <t>Id</t>
   </si>
@@ -392,6 +392,24 @@
     <t>tQI9hKkM1V</t>
   </si>
   <si>
+    <t>Duy2</t>
+  </si>
+  <si>
+    <t>duyduyduy</t>
+  </si>
+  <si>
+    <t>duyduyduy@gmail.com</t>
+  </si>
+  <si>
+    <t>$2y$10$HlCtr3OvtqVBUl6SWRTzTe74SfuCPgfDllOp8h4IuF6NajIoSz1ry</t>
+  </si>
+  <si>
+    <t>08:37 12-03-2020</t>
+  </si>
+  <si>
+    <t>2020-03-12 08:37:52</t>
+  </si>
+  <si>
     <t>Duy</t>
   </si>
   <si>
@@ -401,25 +419,13 @@
     <t>duyduy@gmail.com</t>
   </si>
   <si>
-    <t>$2y$10$Q733oqIih3Eu6YlGy/GLv.VloT/jYB08lXO83fucgyWQuC6o8nln6</t>
-  </si>
-  <si>
-    <t>05:01 12-03-2020</t>
-  </si>
-  <si>
-    <t>2020-03-12 05:01:07</t>
-  </si>
-  <si>
-    <t>Duy2</t>
-  </si>
-  <si>
-    <t>duyduyduy</t>
-  </si>
-  <si>
-    <t>duyduyduy@gmail.com</t>
-  </si>
-  <si>
-    <t>$2y$10$gbKs9qF8PTu5F55L.5L0Xe/owbxllYK7j6eXfwz9QASZeGew269Yy</t>
+    <t>$2y$10$apFWi/SlbxN15H1DS8oNsOyb0dDNXhM.h4KJNYP83NsuqDiKbcvmO</t>
+  </si>
+  <si>
+    <t>09:08 12-03-2020</t>
+  </si>
+  <si>
+    <t>2020-03-12 09:08:55</t>
   </si>
 </sst>
 </file>
@@ -1512,7 +1518,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
         <v>125</v>
@@ -1541,7 +1547,7 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>131</v>
@@ -1561,10 +1567,10 @@
       </c>
       <c r="H24"/>
       <c r="I24" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="J24" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="K24"/>
     </row>

</xml_diff>